<commit_message>
Excel Data driven Class2
</commit_message>
<xml_diff>
--- a/Project_188_Online/TestData/BOOK.xlsx
+++ b/Project_188_Online/TestData/BOOK.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20055" windowHeight="9225"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="20055" windowHeight="9225" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Numerics" sheetId="2" r:id="rId2"/>
+    <sheet name="multiple" sheetId="3" r:id="rId3"/>
+    <sheet name="Conditions" sheetId="4" r:id="rId4"/>
+    <sheet name="mixeddata" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="63">
   <si>
     <t>Application Url</t>
   </si>
@@ -24,16 +26,187 @@
     <t>BrowserName</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>http://google1.v1.com</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
-    <t>Headless</t>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Hello1234</t>
+  </si>
+  <si>
+    <t>http://facebook.com</t>
+  </si>
+  <si>
+    <t>headless</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>Sunil@gmail.com</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Iphone</t>
+  </si>
+  <si>
+    <t>ProductID</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Contant Number</t>
+  </si>
+  <si>
+    <t>9030248855</t>
+  </si>
+  <si>
+    <t>To convert Numeric to Stringcell add single quote before numeric value</t>
+  </si>
+  <si>
+    <t>Data value</t>
+  </si>
+  <si>
+    <t>Boolean value</t>
+  </si>
+  <si>
+    <t>Praveen1</t>
+  </si>
+  <si>
+    <t>Praveen2</t>
+  </si>
+  <si>
+    <t>Praveen3</t>
+  </si>
+  <si>
+    <t>Praveen4</t>
+  </si>
+  <si>
+    <t>Praveen5</t>
+  </si>
+  <si>
+    <t>Praveen6</t>
+  </si>
+  <si>
+    <t>Praveen7</t>
+  </si>
+  <si>
+    <t>Praveen8</t>
+  </si>
+  <si>
+    <t>Praveen9</t>
+  </si>
+  <si>
+    <t>Praveen10</t>
+  </si>
+  <si>
+    <t>Praveen11</t>
+  </si>
+  <si>
+    <t>Praveen12</t>
+  </si>
+  <si>
+    <t>Praveen13</t>
+  </si>
+  <si>
+    <t>Praveen14</t>
+  </si>
+  <si>
+    <t>Praveen15</t>
+  </si>
+  <si>
+    <t>Praveen16</t>
+  </si>
+  <si>
+    <t>Praveen17</t>
+  </si>
+  <si>
+    <t>Praveen18</t>
+  </si>
+  <si>
+    <t>New_prv_1</t>
+  </si>
+  <si>
+    <t>New_prv_2</t>
+  </si>
+  <si>
+    <t>New_prv_3</t>
+  </si>
+  <si>
+    <t>New_prv_4</t>
+  </si>
+  <si>
+    <t>New_prv_5</t>
+  </si>
+  <si>
+    <t>New_prv_6</t>
+  </si>
+  <si>
+    <t>New_prv_7</t>
+  </si>
+  <si>
+    <t>New_prv_8</t>
+  </si>
+  <si>
+    <t>New_prv_9</t>
+  </si>
+  <si>
+    <t>New_prv_10</t>
+  </si>
+  <si>
+    <t>New_prv_11</t>
+  </si>
+  <si>
+    <t>New_prv_12</t>
+  </si>
+  <si>
+    <t>New_prv_13</t>
+  </si>
+  <si>
+    <t>New_prv_14</t>
+  </si>
+  <si>
+    <t>New_prv_15</t>
+  </si>
+  <si>
+    <t>New_prv_16</t>
+  </si>
+  <si>
+    <t>New_prv_17</t>
+  </si>
+  <si>
+    <t>New_prv_18</t>
+  </si>
+  <si>
+    <t>Praveen19</t>
+  </si>
+  <si>
+    <t>New_prv_19</t>
+  </si>
+  <si>
+    <t>Praveen20</t>
+  </si>
+  <si>
+    <t>New_prv_20</t>
+  </si>
+  <si>
+    <t>Execution_Status</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -56,7 +229,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -66,6 +239,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -86,10 +265,19 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -385,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -406,23 +594,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -430,24 +635,702 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+    <col min="6" max="6" width="52.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>1002345675</v>
+      </c>
+      <c r="C2">
+        <v>25000.12</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45">
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="5">
+        <v>44542</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6">
+        <v>12345</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="7"/>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="6">
+        <v>12345</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>